<commit_message>
improved code, fixed family members, view xml fucntion added
</commit_message>
<xml_diff>
--- a/EPO/output.xlsx
+++ b/EPO/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Patent No.</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Family Id</t>
   </si>
   <si>
+    <t>Application Date</t>
+  </si>
+  <si>
     <t>Earliest priority</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
     <t>Assignee</t>
   </si>
   <si>
+    <t>Inventors</t>
+  </si>
+  <si>
     <t>Family members</t>
   </si>
   <si>
@@ -47,49 +53,19 @@
     <t>38896881</t>
   </si>
   <si>
+    <t>20061122</t>
+  </si>
+  <si>
     <t>20120320</t>
   </si>
   <si>
     <t xml:space="preserve">OSHKOSH TRUCK CORPORATION, </t>
   </si>
   <si>
-    <t>US2007291130A1| US2007291130A1| US8139109B2| US8139109B2| CA2724324A1| CA2724324A1| CA2724324C| CA2724324C| GB201020969D0| GB201020969D0| GB2473379A| GB2473379A| GB2473379B| GB2473379B| US2009079839A1| US2009079839A1| US8947531B2| US8947531B2| US2012143430A1| US2012143430A1| US9420203B2| US9420203B2| WO2008073518A2| WO2008073518A2| WO2008073518A3| WO2008073518A3| WO2009140514A2| WO2009140514A2| WO2009140514A3| WO2009140514A3</t>
-  </si>
-  <si>
-    <t>US5606609A</t>
-  </si>
-  <si>
-    <t>Electronic document verification system and method</t>
-  </si>
-  <si>
-    <t>23185324</t>
-  </si>
-  <si>
-    <t>19970225</t>
-  </si>
-  <si>
-    <t>SCIENTIFIC-ATLANTA</t>
-  </si>
-  <si>
-    <t>US5606609A| US5606609A</t>
-  </si>
-  <si>
-    <t>EP1417800B1</t>
-  </si>
-  <si>
-    <t>METHOD AND SYSTEM FOR STORING LARGE DATA FILES</t>
-  </si>
-  <si>
-    <t>27129973</t>
-  </si>
-  <si>
-    <t>20171004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENTLEY SYSTEMS, INCORPORATED, </t>
-  </si>
-  <si>
-    <t>EP1417800A1| EP1417800A1| EP1417800A4| EP1417800A4| EP1417800B1| EP1417800B1| DK1417800T3| DK1417800T3| EP2597811A1| EP2597811A1| EP2597811B1| EP2597811B1| US2003037182A1| US2003037182A1| US7162479B2| US7162479B2| US2003036888A1| US2003036888A1| US7428548B2| US7428548B2| US2007192376A1| US2007192376A1| US7743080B2| US7743080B2| WO03017567A1| WO03017567A1</t>
+    <t>BROGGI ALBERTO, | SCHMIEDEL GARY, | YAKES CHRISTOPHER K</t>
+  </si>
+  <si>
+    <t>US8947531B2| GB2473379A| GB2473379B| WO2008073518A2| CA2724324C| US2007291130A1| WO2009140514A3| WO2009140514A2| US8139109B2| CA2724324A1| US2012143430A1| GB201020969D0| US9420203B2| WO2008073518A3| US2009079839A1</t>
   </si>
 </sst>
 </file>
@@ -438,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +422,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,83 +444,43 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="n">
         <v>20060619</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="n">
-        <v>19940919</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="J2" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20010815</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code improved, bugs fixed
</commit_message>
<xml_diff>
--- a/EPO/output.xlsx
+++ b/EPO/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Patent No.</t>
   </si>
@@ -44,28 +44,97 @@
     <t>Family members</t>
   </si>
   <si>
-    <t>US8139109B2</t>
-  </si>
-  <si>
-    <t>Vision system for an autonomous vehicle</t>
-  </si>
-  <si>
-    <t>38896881</t>
-  </si>
-  <si>
-    <t>20061122</t>
-  </si>
-  <si>
-    <t>20120320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OSHKOSH TRUCK CORPORATION, </t>
-  </si>
-  <si>
-    <t>BROGGI ALBERTO, | SCHMIEDEL GARY, | YAKES CHRISTOPHER K</t>
-  </si>
-  <si>
-    <t>US8947531B2| GB2473379A| GB2473379B| WO2008073518A2| CA2724324C| US2007291130A1| WO2009140514A3| WO2009140514A2| US8139109B2| CA2724324A1| US2012143430A1| GB201020969D0| US9420203B2| WO2008073518A3| US2009079839A1</t>
+    <t>US20020107833A1</t>
+  </si>
+  <si>
+    <t>Method and system for tracking equipment usage information</t>
+  </si>
+  <si>
+    <t>22585439</t>
+  </si>
+  <si>
+    <t>20011116</t>
+  </si>
+  <si>
+    <t>20020808</t>
+  </si>
+  <si>
+    <t>KERKINNI FUAT J</t>
+  </si>
+  <si>
+    <t>KERKINNI FUAT</t>
+  </si>
+  <si>
+    <t>US2002107833A1| AU2619801A| WO0135679A3| WO0135679A2</t>
+  </si>
+  <si>
+    <t>JP2002196817A</t>
+  </si>
+  <si>
+    <t>SYSTEM FOR MANAGING WORK VEHICLE</t>
+  </si>
+  <si>
+    <t>18859294</t>
+  </si>
+  <si>
+    <t>20001225</t>
+  </si>
+  <si>
+    <t>20020712</t>
+  </si>
+  <si>
+    <t>ISEKI &amp; CO LTD</t>
+  </si>
+  <si>
+    <t>IKEUCHI NOBUAKI, WATABE TOMOAKI, SHINODA MASANORI, SAKATA CHIKANO</t>
+  </si>
+  <si>
+    <t>US6434512B1</t>
+  </si>
+  <si>
+    <t>Modular data collection and analysis system</t>
+  </si>
+  <si>
+    <t>27489613</t>
+  </si>
+  <si>
+    <t>19990930</t>
+  </si>
+  <si>
+    <t>20020813</t>
+  </si>
+  <si>
+    <t>RELIANCE ELECTRIC TECHNOLOGIES, LLC</t>
+  </si>
+  <si>
+    <t>DISCENZO FREDERICK</t>
+  </si>
+  <si>
+    <t>US7690246B1| US6546785B1| US7493799B1| US6877360B1| US6286363B1| US6434512B1| US6023961A| US6196057B1| US7134323B1| US6295510B1| US6324899B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> US20020111725A1</t>
+  </si>
+  <si>
+    <t>Method and apparatus for risk-related use of vehicle communication system data</t>
+  </si>
+  <si>
+    <t>27575201</t>
+  </si>
+  <si>
+    <t>20010716</t>
+  </si>
+  <si>
+    <t>20020815</t>
+  </si>
+  <si>
+    <t>BURGE JOHN R</t>
+  </si>
+  <si>
+    <t>BURGE JOHN</t>
+  </si>
+  <si>
+    <t>US2002103622A1| US2002111725A1</t>
   </si>
 </sst>
 </file>
@@ -414,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +537,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>20060619</v>
+        <v>19991029</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -481,6 +550,102 @@
       </c>
       <c r="J2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20001225</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="n">
+        <v>19980402</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="n">
+        <v>20000717</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>